<commit_message>
BBS board list & board insert & reply
</commit_message>
<xml_diff>
--- a/bbs_routing.xlsx
+++ b/bbs_routing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>routing</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -239,6 +239,58 @@
   </si>
   <si>
     <t>p=1, f, q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/board/detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bid, uid, option</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board, replyList, fileList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/WEB-INF/view/board/detail.j네</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/reply/write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bid, uid, comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bid, uid, option=DNI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/file/download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/file/profile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -395,14 +447,14 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -688,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -731,11 +783,11 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1"/>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="17.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33">
+    <row r="4" spans="1:7" ht="49.5">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
@@ -757,7 +809,7 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -774,7 +826,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="33">
-      <c r="A6" s="7"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -793,7 +845,7 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -810,7 +862,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="7"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
@@ -831,7 +883,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -846,7 +898,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -865,11 +917,11 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="34.5">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -927,7 +979,7 @@
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" ht="17.25"/>
     <row r="16" spans="1:7" ht="17.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -953,43 +1005,121 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="7" t="s">
-        <v>36</v>
+      <c r="A18" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="7"/>
+      <c r="A19" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="B19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>53</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="10"/>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25">
+      <c r="A23" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="27" spans="1:7" ht="17.25">
+      <c r="A27" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Maven BBS Reply update
</commit_message>
<xml_diff>
--- a/bbs_routing.xlsx
+++ b/bbs_routing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="105">
   <si>
     <t>routing</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>uid, uname, email, addr, profile, filename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">/WEB-INF/view/user/delete.jsp </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -182,10 +178,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">/WEB-INF/view/board/write.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/bbs/user</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -210,10 +202,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>uid, uname, email, profile, addr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>page, userList, pageList,  totalPages, startPage, endPage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -282,10 +270,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">/WEB-INF/view/board/detail.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>bid, uid, f, q, option</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -346,18 +330,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">/WEB-INF/view/board/update.jsp </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>field, query</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>bid, currentBoardPage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>p, f, q</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -371,6 +343,106 @@
   </si>
   <si>
     <t>한글은 엔코딩할 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid, uname, email, profile, addr, stateMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid, uname, email, addr, profile, filename, hashedPwd, pwd, pwd2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>msg, url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/WEB-INF/view/common/alertMsg.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">msg: 이름, url: /bbs/board/list?p=currentUserPage(세션값)&amp;f=&amp;q= </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page=currentUserPage(세션값), 패스워드 변경 안 할 때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/WEB-INF/view/board/detailEditor.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/WEB-INF/view/board/writeEditor.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/WEB-INF/view/board/updateEditor.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bid, f, q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bid, currentBoardPage, f, q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">/WEB-INF/view/error/error404.jsp </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/fileimageUpload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CKEditorFuncNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file download</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로파일 이미지 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ckeditor 이미지 다운로드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/aside</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bbs/aside/stateMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stateMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ajaxResponse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"0"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -378,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,13 +471,6 @@
       <color theme="0"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -437,7 +502,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -446,8 +511,32 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -473,7 +562,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -497,14 +586,42 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -514,50 +631,65 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -841,467 +973,646 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="41.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="20.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="81" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1"/>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="17.25">
-      <c r="A3" s="8" t="s">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="49.5">
-      <c r="A4" s="5" t="s">
+      <c r="B9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="E11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="94.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="33">
-      <c r="A6" s="10"/>
-      <c r="B6" s="5" t="s">
+      <c r="F18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" ht="54" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" ht="27" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="10"/>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="34.5">
-      <c r="A11" s="10"/>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" ht="17.25"/>
-    <row r="16" spans="1:7" ht="17.25">
-      <c r="A16" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="66">
-      <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="C29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="E29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="33">
-      <c r="A18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="10"/>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="14"/>
-      <c r="B22" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17.25">
-      <c r="A27" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="C34" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="17.25">
-      <c r="A31" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+    </row>
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>